<commit_message>
Move template version to ConceptScheme sheet
</commit_message>
<xml_diff>
--- a/src/voc4cat/templates/vocab/blank_043.xlsx
+++ b/src/voc4cat/templates/vocab/blank_043.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\MyProg\gh-nfdi4cat\voc4cat\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-tool\src\voc4cat\templates\vocab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCFAF9A-16AB-4F1A-9E10-106FA17068AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1209A9-5678-4E59-91D2-38A6DB0E7FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="8700" windowWidth="28500" windowHeight="8535" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9495" yWindow="5475" windowWidth="28800" windowHeight="15825" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="90">
   <si>
     <t>Template version</t>
   </si>
@@ -1474,6 +1474,15 @@
       </rPr>
       <t xml:space="preserve"> = A catalogue PID or DOI, e.g. eCat ID, if the vocab has one.</t>
     </r>
+  </si>
+  <si>
+    <t>Template Version</t>
+  </si>
+  <si>
+    <t>Version of the xlsx template</t>
+  </si>
+  <si>
+    <t>0.4.3, rev. 2025-07a</t>
   </si>
 </sst>
 </file>
@@ -2343,7 +2352,9 @@
   </sheetPr>
   <dimension ref="A11:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11:J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5211,7 +5222,7 @@
   <dimension ref="A1:D994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5359,7 +5370,20 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update help sheet in xlsx template 0.43 for Parent IRIs
</commit_message>
<xml_diff>
--- a/src/voc4cat/templates/vocab/blank_043.xlsx
+++ b/src/voc4cat/templates/vocab/blank_043.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\MyProg\gh-nfdi4cat\voc4cat-tool\src\voc4cat\templates\vocab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB2DD96-B9D9-45E2-8176-7A686974A8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409C6B20-187D-4A0D-9612-FA30AA5F24C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="8280" windowWidth="28260" windowHeight="9120" tabRatio="652" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="1170" windowWidth="28260" windowHeight="16380" tabRatio="652" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
-    <sheet name="Help" sheetId="8" r:id="rId2"/>
+    <sheet name="Help" sheetId="9" r:id="rId2"/>
     <sheet name="Concept Scheme" sheetId="3" r:id="rId3"/>
     <sheet name="Concepts" sheetId="4" r:id="rId4"/>
     <sheet name="Additional Concept Features" sheetId="5" r:id="rId5"/>
@@ -284,9 +284,6 @@
     <t>Namespace</t>
   </si>
   <si>
-    <t>2025-02a</t>
-  </si>
-  <si>
     <t>Voc4Cat online help &amp; guidelines</t>
   </si>
   <si>
@@ -490,7 +487,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Concepts (mandatory)</t>
+      <t>Prefix Sheet</t>
     </r>
     <r>
       <rPr>
@@ -513,6 +510,498 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>This sheet shows the known mappings between short prefixes and namespaces which are the basis for using "compact URI" also called "CURIE". This sheet is write only; any changes will be ignored. For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
+Example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: http://example.org/1, http://example.org/2, http://example.org/3</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Instead of manually typing out said examples, you can add in the Prefix Sheet a "ex" as Prefix, and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "http://example.org/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" as the corresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Finally...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+After completing this sheet, you can process it locally with the voc4cat command line tool. To get more information about how to install and use it, visit https://github.com/nfdi4cat/voc4cat-tool/. Alternatively you may want to submit the xlsx file as a pull request to a voc4cat-enabled repository such as</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Concept Scheme (mandatory)</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The Concept Scheme sheet collects the top level information about the vocabulary.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Vocabulary IRI* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= The IRI that refers to this specific vocabulary. It must be a valid URI. For testing you can first use a fake value, as long as it's a valid URI, and replace it later (e.g. http://example.com/def/v1 ). 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: An IRI (International Resource Identifier) is like a URI (Uniform Reference Identifier) but with more permissible characters. Note: Instead of a full IRI you can use a CURIE (compact URI) defined with the prefix sheet, e.g. ex:v1 where "ex" stands for the namespace "http://example.com/def/". See below for more on the Prefix Sheet.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Title*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =  A short one line title for the vocabulary.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A general description for the vocabulary and its scope. This can be as long as needed and may contain all possible characters and line breaks.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Created Date*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The vocabulary's creation date.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Modified Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The vocabulary's latest modification date (optional).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: Dates in these cells must be recognized as date by Excel but may be in localized format.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Creator*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A ROR ID, an ORCID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Publisher*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A ROR ID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Either the abbreviation for an organization or its URI can be given. The organization abbreviation is validated against a predefined list of organizations. If you miss an organization, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition (or just use a ROR ID!).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A version specifier for this vocabulary, e.g. v2022-02-22 (it is suggested to use calendar-based versioning).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Versions strings should start with "v" to prevent Excel from interpreting it as number of date.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provenance*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A note on the source of this vocabulary. This should be an identifier for the person and a provenance note. As identifier, an ORCID ID (with or without https://orcid.org/ part) or a GitHub name should be used. Multiple entries must be separated with a comma. For provenance fields there is no strict validation in place because handling of provenance is still in discussion, see https://github.com/nfdi4cat/voc4cat-tool/issues/122
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Custodian</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The person managing this vocabulary's content, e.g. "Sofia Garcia (orcid:0000-0001-2345-6789)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Catalogue PID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A catalogue PID or DOI, e.g. eCat ID, if the vocab has one.</t>
+    </r>
+  </si>
+  <si>
+    <t>Template Version</t>
+  </si>
+  <si>
+    <t>Version of the xlsx template</t>
+  </si>
+  <si>
+    <t>0.4.3, rev. 2025-07a</t>
+  </si>
+  <si>
+    <t>Parent IRIs</t>
+  </si>
+  <si>
+    <t>2025-07a</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Concepts (mandatory)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">A concept according to SKOS is a unit of thought, idea, meaning, or category of an object or event which underlies a knowledge organization system. This sheet collects concept descriptions, (optionally) their translations to other languages, simple broader/ narrower relations between the concepts and provenance information.
 </t>
     </r>
@@ -602,7 +1091,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> = Two or three letter language code according to ISO 639-2 or 639-3 for the Preferred Label  (see https://iso639-3.sil.org/code_tables/639/data).  If no language code is given, "en" is assumed as default.
-With voc4cat you may use indentation of the Preferred Label (xlsx-indentation or character-based indentation) to express parent-child (broader/narrower) relations between concepts. If you use indentation, the Children IRIs column (see below) is ignored. voc4cat allows to convert in both directions between indentation-based and Children-IRIs-based representation.
 </t>
     </r>
     <r>
@@ -723,16 +1211,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Children URIs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A list of IRIs of children of this Concept, separated by commas. This creates a hierarchical relationship between the terms. In SKOS terminology, the Concept is broader than its Concept-Child and in turn the Concept-Child is narrower than the Concept. </t>
+      <t>Parent IRIs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A list of IRIs of parents of this Concept, separated by commas. This creates a hierarchical relationship between the terms. In SKOS terminology, the Concept is narrower than its Concept-Parent and in turn the Concept-Parent is broader than the Concept. </t>
     </r>
     <r>
       <rPr>
@@ -992,497 +1480,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note on Broader/Narrower: In sheet "Concepts" broader/narrower is expressed via "Children URIs" or as indentation. The broader/narrower columns in this sheet should be used to express broader/narrower relations with external concepts.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Prefix Sheet</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This sheet shows the known mappings between short prefixes and namespaces which are the basis for using "compact URI" also called "CURIE". This sheet is write only; any changes will be ignored. For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
-Example</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: http://example.org/1, http://example.org/2, http://example.org/3</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Instead of manually typing out said examples, you can add in the Prefix Sheet a "ex" as Prefix, and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "http://example.org/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" as the corresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Finally...</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-After completing this sheet, you can process it locally with the voc4cat command line tool. To get more information about how to install and use it, visit https://github.com/nfdi4cat/voc4cat-tool/. Alternatively you may want to submit the xlsx file as a pull request to a voc4cat-enabled repository such as</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Concept Scheme (mandatory)</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The Concept Scheme sheet collects the top level information about the vocabulary.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Vocabulary IRI* </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= The IRI that refers to this specific vocabulary. It must be a valid URI. For testing you can first use a fake value, as long as it's a valid URI, and replace it later (e.g. http://example.com/def/v1 ). 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Note: An IRI (International Resource Identifier) is like a URI (Uniform Reference Identifier) but with more permissible characters. Note: Instead of a full IRI you can use a CURIE (compact URI) defined with the prefix sheet, e.g. ex:v1 where "ex" stands for the namespace "http://example.com/def/". See below for more on the Prefix Sheet.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Title*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =  A short one line title for the vocabulary.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Description*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A general description for the vocabulary and its scope. This can be as long as needed and may contain all possible characters and line breaks.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Created Date*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The vocabulary's creation date.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Modified Date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The vocabulary's latest modification date (optional).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Note: Dates in these cells must be recognized as date by Excel but may be in localized format.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Creator*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A ROR ID, an ORCID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Publisher*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A ROR ID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: Either the abbreviation for an organization or its URI can be given. The organization abbreviation is validated against a predefined list of organizations. If you miss an organization, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition (or just use a ROR ID!).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Version</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A version specifier for this vocabulary, e.g. v2022-02-22 (it is suggested to use calendar-based versioning).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: Versions strings should start with "v" to prevent Excel from interpreting it as number of date.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Provenance*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A note on the source of this vocabulary. This should be an identifier for the person and a provenance note. As identifier, an ORCID ID (with or without https://orcid.org/ part) or a GitHub name should be used. Multiple entries must be separated with a comma. For provenance fields there is no strict validation in place because handling of provenance is still in discussion, see https://github.com/nfdi4cat/voc4cat-tool/issues/122
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Custodian</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The person managing this vocabulary's content, e.g. "Sofia Garcia (orcid:0000-0001-2345-6789)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Catalogue PID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A catalogue PID or DOI, e.g. eCat ID, if the vocab has one.</t>
-    </r>
-  </si>
-  <si>
-    <t>Template Version</t>
-  </si>
-  <si>
-    <t>Version of the xlsx template</t>
-  </si>
-  <si>
-    <t>0.4.3, rev. 2025-07a</t>
-  </si>
-  <si>
-    <t>Parent IRIs</t>
+      <t>Note on Broader/Narrower: In sheet "Concepts" broader/narrower is expressed via "Parent IRIs". The broader/narrower columns in this sheet should be used to express broader/narrower relations with external concepts.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1748,11 +1747,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1839,6 +1835,10 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2353,7 +2353,7 @@
   <dimension ref="A11:L32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:J12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2363,141 +2363,141 @@
   </cols>
   <sheetData>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H12" s="9"/>
-      <c r="I12" s="10" t="s">
+      <c r="H12" s="8"/>
+      <c r="I12" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="11" t="s">
-        <v>68</v>
+      <c r="J12" s="10" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
+      <c r="B14" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="L16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="L17" s="12"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="L17" s="11"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D23" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D24" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D25" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="34" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D23" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D24" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D25" s="13" t="s">
+      <c r="E25" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="26" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D26" s="13"/>
+      <c r="D26" s="12"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D28" s="13"/>
-      <c r="E28" s="14" t="s">
+      <c r="D28" s="12"/>
+      <c r="E28" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2507,10 +2507,10 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2534,1612 +2534,1617 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACB5065-711E-402F-8A08-0C72FAF4F712}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BBBF83-22D1-45C1-8A61-DBB84058260B}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J1169"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="12.5703125" style="36"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
+      <c r="B12" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
     </row>
     <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
     </row>
     <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
     </row>
     <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
     </row>
     <row r="21" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
     </row>
     <row r="22" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
     </row>
     <row r="23" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
     </row>
     <row r="24" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
     </row>
     <row r="25" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
     </row>
     <row r="26" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
     </row>
     <row r="27" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
     </row>
     <row r="31" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
     </row>
     <row r="32" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
     </row>
     <row r="33" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
     </row>
     <row r="34" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
     </row>
     <row r="35" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
     </row>
     <row r="36" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="36"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="37"/>
     </row>
     <row r="37" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
     </row>
     <row r="38" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
     </row>
     <row r="39" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
     </row>
     <row r="40" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
     </row>
     <row r="41" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
     </row>
     <row r="42" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
     </row>
     <row r="43" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
     </row>
     <row r="44" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
     </row>
     <row r="45" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
     </row>
     <row r="48" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B48" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="36"/>
+      <c r="B48" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
     </row>
     <row r="49" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="36"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
     </row>
     <row r="50" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="36"/>
-      <c r="J50" s="36"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
     </row>
     <row r="51" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="36"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
     </row>
     <row r="52" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="36"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
     </row>
     <row r="53" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="36"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
     </row>
     <row r="54" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="36"/>
-      <c r="J54" s="36"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
     </row>
     <row r="55" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="36"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
     </row>
     <row r="56" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="36"/>
-      <c r="J56" s="36"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
     </row>
     <row r="57" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="36"/>
-      <c r="J57" s="36"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
     </row>
     <row r="58" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="36"/>
-      <c r="J58" s="36"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
     </row>
     <row r="59" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="36"/>
-      <c r="J59" s="36"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
     </row>
     <row r="60" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="36"/>
-      <c r="J60" s="36"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
     </row>
     <row r="61" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="36"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
     </row>
     <row r="62" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="36"/>
-      <c r="J62" s="36"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="37"/>
     </row>
     <row r="63" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="36"/>
-      <c r="H63" s="36"/>
-      <c r="I63" s="36"/>
-      <c r="J63" s="36"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="37"/>
     </row>
     <row r="64" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="36"/>
-      <c r="H64" s="36"/>
-      <c r="I64" s="36"/>
-      <c r="J64" s="36"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
     </row>
     <row r="65" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="36"/>
-      <c r="H65" s="36"/>
-      <c r="I65" s="36"/>
-      <c r="J65" s="36"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="37"/>
+      <c r="J65" s="37"/>
     </row>
     <row r="66" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
-      <c r="F66" s="36"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="36"/>
-      <c r="I66" s="36"/>
-      <c r="J66" s="36"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="37"/>
+      <c r="J66" s="37"/>
     </row>
     <row r="67" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="36"/>
-      <c r="H67" s="36"/>
-      <c r="I67" s="36"/>
-      <c r="J67" s="36"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
     </row>
     <row r="68" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
-      <c r="F68" s="36"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="36"/>
-      <c r="I68" s="36"/>
-      <c r="J68" s="36"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
     </row>
     <row r="69" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="36"/>
-      <c r="F69" s="36"/>
-      <c r="G69" s="36"/>
-      <c r="H69" s="36"/>
-      <c r="I69" s="36"/>
-      <c r="J69" s="36"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="37"/>
     </row>
     <row r="70" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="36"/>
-      <c r="G70" s="36"/>
-      <c r="H70" s="36"/>
-      <c r="I70" s="36"/>
-      <c r="J70" s="36"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="37"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="37"/>
+      <c r="J70" s="37"/>
     </row>
     <row r="71" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B71" s="36"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
-      <c r="H71" s="36"/>
-      <c r="I71" s="36"/>
-      <c r="J71" s="36"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
+      <c r="J71" s="37"/>
     </row>
     <row r="72" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
-      <c r="G72" s="36"/>
-      <c r="H72" s="36"/>
-      <c r="I72" s="36"/>
-      <c r="J72" s="36"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
+      <c r="G72" s="37"/>
+      <c r="H72" s="37"/>
+      <c r="I72" s="37"/>
+      <c r="J72" s="37"/>
     </row>
     <row r="73" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B73" s="36"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="36"/>
-      <c r="G73" s="36"/>
-      <c r="H73" s="36"/>
-      <c r="I73" s="36"/>
-      <c r="J73" s="36"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="37"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="37"/>
     </row>
     <row r="74" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="36"/>
-      <c r="I74" s="36"/>
-      <c r="J74" s="36"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="37"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37"/>
+      <c r="J74" s="37"/>
     </row>
     <row r="75" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
-      <c r="G75" s="36"/>
-      <c r="H75" s="36"/>
-      <c r="I75" s="36"/>
-      <c r="J75" s="36"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="37"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="37"/>
+      <c r="G75" s="37"/>
+      <c r="H75" s="37"/>
+      <c r="I75" s="37"/>
+      <c r="J75" s="37"/>
     </row>
     <row r="76" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B76" s="36"/>
-      <c r="C76" s="36"/>
-      <c r="D76" s="36"/>
-      <c r="E76" s="36"/>
-      <c r="F76" s="36"/>
-      <c r="G76" s="36"/>
-      <c r="H76" s="36"/>
-      <c r="I76" s="36"/>
-      <c r="J76" s="36"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="37"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="37"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="37"/>
+      <c r="I76" s="37"/>
+      <c r="J76" s="37"/>
     </row>
     <row r="77" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B77" s="36"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="36"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="36"/>
-      <c r="G77" s="36"/>
-      <c r="H77" s="36"/>
-      <c r="I77" s="36"/>
-      <c r="J77" s="36"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="37"/>
+      <c r="G77" s="37"/>
+      <c r="H77" s="37"/>
+      <c r="I77" s="37"/>
+      <c r="J77" s="37"/>
     </row>
     <row r="78" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B78" s="36"/>
-      <c r="C78" s="36"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="36"/>
-      <c r="G78" s="36"/>
-      <c r="H78" s="36"/>
-      <c r="I78" s="36"/>
-      <c r="J78" s="36"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="37"/>
+      <c r="H78" s="37"/>
+      <c r="I78" s="37"/>
+      <c r="J78" s="37"/>
     </row>
     <row r="79" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B79" s="36"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="36"/>
-      <c r="F79" s="36"/>
-      <c r="G79" s="36"/>
-      <c r="H79" s="36"/>
-      <c r="I79" s="36"/>
-      <c r="J79" s="36"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="37"/>
+      <c r="G79" s="37"/>
+      <c r="H79" s="37"/>
+      <c r="I79" s="37"/>
+      <c r="J79" s="37"/>
     </row>
     <row r="80" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B80" s="36"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="36"/>
-      <c r="F80" s="36"/>
-      <c r="G80" s="36"/>
-      <c r="H80" s="36"/>
-      <c r="I80" s="36"/>
-      <c r="J80" s="36"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="37"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="37"/>
+      <c r="G80" s="37"/>
+      <c r="H80" s="37"/>
+      <c r="I80" s="37"/>
+      <c r="J80" s="37"/>
     </row>
     <row r="81" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
-      <c r="F81" s="36"/>
-      <c r="G81" s="36"/>
-      <c r="H81" s="36"/>
-      <c r="I81" s="36"/>
-      <c r="J81" s="36"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="37"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="37"/>
+      <c r="G81" s="37"/>
+      <c r="H81" s="37"/>
+      <c r="I81" s="37"/>
+      <c r="J81" s="37"/>
     </row>
     <row r="82" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B82" s="36"/>
-      <c r="C82" s="36"/>
-      <c r="D82" s="36"/>
-      <c r="E82" s="36"/>
-      <c r="F82" s="36"/>
-      <c r="G82" s="36"/>
-      <c r="H82" s="36"/>
-      <c r="I82" s="36"/>
-      <c r="J82" s="36"/>
+      <c r="B82" s="37"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="37"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="37"/>
+      <c r="I82" s="37"/>
+      <c r="J82" s="37"/>
     </row>
     <row r="83" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B83" s="36"/>
-      <c r="C83" s="36"/>
-      <c r="D83" s="36"/>
-      <c r="E83" s="36"/>
-      <c r="F83" s="36"/>
-      <c r="G83" s="36"/>
-      <c r="H83" s="36"/>
-      <c r="I83" s="36"/>
-      <c r="J83" s="36"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="37"/>
+      <c r="E83" s="37"/>
+      <c r="F83" s="37"/>
+      <c r="G83" s="37"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="37"/>
+      <c r="J83" s="37"/>
     </row>
     <row r="84" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
-      <c r="F84" s="36"/>
-      <c r="G84" s="36"/>
-      <c r="H84" s="36"/>
-      <c r="I84" s="36"/>
-      <c r="J84" s="36"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="37"/>
+      <c r="G84" s="37"/>
+      <c r="H84" s="37"/>
+      <c r="I84" s="37"/>
+      <c r="J84" s="37"/>
     </row>
     <row r="85" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B85" s="36"/>
-      <c r="C85" s="36"/>
-      <c r="D85" s="36"/>
-      <c r="E85" s="36"/>
-      <c r="F85" s="36"/>
-      <c r="G85" s="36"/>
-      <c r="H85" s="36"/>
-      <c r="I85" s="36"/>
-      <c r="J85" s="36"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="37"/>
+      <c r="G85" s="37"/>
+      <c r="H85" s="37"/>
+      <c r="I85" s="37"/>
+      <c r="J85" s="37"/>
     </row>
     <row r="86" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B86" s="36"/>
-      <c r="C86" s="36"/>
-      <c r="D86" s="36"/>
-      <c r="E86" s="36"/>
-      <c r="F86" s="36"/>
-      <c r="G86" s="36"/>
-      <c r="H86" s="36"/>
-      <c r="I86" s="36"/>
-      <c r="J86" s="36"/>
+      <c r="B86" s="37"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="37"/>
+      <c r="G86" s="37"/>
+      <c r="H86" s="37"/>
+      <c r="I86" s="37"/>
+      <c r="J86" s="37"/>
     </row>
     <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B87" s="36"/>
-      <c r="C87" s="36"/>
-      <c r="D87" s="36"/>
-      <c r="E87" s="36"/>
-      <c r="F87" s="36"/>
-      <c r="G87" s="36"/>
-      <c r="H87" s="36"/>
-      <c r="I87" s="36"/>
-      <c r="J87" s="36"/>
+      <c r="B87" s="37"/>
+      <c r="C87" s="37"/>
+      <c r="D87" s="37"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="37"/>
+      <c r="H87" s="37"/>
+      <c r="I87" s="37"/>
+      <c r="J87" s="37"/>
     </row>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B88" s="36"/>
-      <c r="C88" s="36"/>
-      <c r="D88" s="36"/>
-      <c r="E88" s="36"/>
-      <c r="F88" s="36"/>
-      <c r="G88" s="36"/>
-      <c r="H88" s="36"/>
-      <c r="I88" s="36"/>
-      <c r="J88" s="36"/>
+      <c r="B88" s="37"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="37"/>
+      <c r="G88" s="37"/>
+      <c r="H88" s="37"/>
+      <c r="I88" s="37"/>
+      <c r="J88" s="37"/>
     </row>
     <row r="89" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="90" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B90" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C90" s="36"/>
-      <c r="D90" s="36"/>
-      <c r="E90" s="36"/>
-      <c r="F90" s="36"/>
-      <c r="G90" s="36"/>
-      <c r="H90" s="36"/>
-      <c r="I90" s="36"/>
-      <c r="J90" s="36"/>
+      <c r="B90" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
+      <c r="E90" s="37"/>
+      <c r="F90" s="37"/>
+      <c r="G90" s="37"/>
+      <c r="H90" s="37"/>
+      <c r="I90" s="37"/>
+      <c r="J90" s="37"/>
     </row>
     <row r="91" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B91" s="36"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="36"/>
-      <c r="E91" s="36"/>
-      <c r="F91" s="36"/>
-      <c r="G91" s="36"/>
-      <c r="H91" s="36"/>
-      <c r="I91" s="36"/>
-      <c r="J91" s="36"/>
+      <c r="B91" s="37"/>
+      <c r="C91" s="37"/>
+      <c r="D91" s="37"/>
+      <c r="E91" s="37"/>
+      <c r="F91" s="37"/>
+      <c r="G91" s="37"/>
+      <c r="H91" s="37"/>
+      <c r="I91" s="37"/>
+      <c r="J91" s="37"/>
     </row>
     <row r="92" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B92" s="36"/>
-      <c r="C92" s="36"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="36"/>
-      <c r="F92" s="36"/>
-      <c r="G92" s="36"/>
-      <c r="H92" s="36"/>
-      <c r="I92" s="36"/>
-      <c r="J92" s="36"/>
+      <c r="B92" s="37"/>
+      <c r="C92" s="37"/>
+      <c r="D92" s="37"/>
+      <c r="E92" s="37"/>
+      <c r="F92" s="37"/>
+      <c r="G92" s="37"/>
+      <c r="H92" s="37"/>
+      <c r="I92" s="37"/>
+      <c r="J92" s="37"/>
     </row>
     <row r="93" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B93" s="36"/>
-      <c r="C93" s="36"/>
-      <c r="D93" s="36"/>
-      <c r="E93" s="36"/>
-      <c r="F93" s="36"/>
-      <c r="G93" s="36"/>
-      <c r="H93" s="36"/>
-      <c r="I93" s="36"/>
-      <c r="J93" s="36"/>
+      <c r="B93" s="37"/>
+      <c r="C93" s="37"/>
+      <c r="D93" s="37"/>
+      <c r="E93" s="37"/>
+      <c r="F93" s="37"/>
+      <c r="G93" s="37"/>
+      <c r="H93" s="37"/>
+      <c r="I93" s="37"/>
+      <c r="J93" s="37"/>
     </row>
     <row r="94" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B94" s="36"/>
-      <c r="C94" s="36"/>
-      <c r="D94" s="36"/>
-      <c r="E94" s="36"/>
-      <c r="F94" s="36"/>
-      <c r="G94" s="36"/>
-      <c r="H94" s="36"/>
-      <c r="I94" s="36"/>
-      <c r="J94" s="36"/>
+      <c r="B94" s="37"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="37"/>
+      <c r="F94" s="37"/>
+      <c r="G94" s="37"/>
+      <c r="H94" s="37"/>
+      <c r="I94" s="37"/>
+      <c r="J94" s="37"/>
     </row>
     <row r="95" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B95" s="36"/>
-      <c r="C95" s="36"/>
-      <c r="D95" s="36"/>
-      <c r="E95" s="36"/>
-      <c r="F95" s="36"/>
-      <c r="G95" s="36"/>
-      <c r="H95" s="36"/>
-      <c r="I95" s="36"/>
-      <c r="J95" s="36"/>
+      <c r="B95" s="37"/>
+      <c r="C95" s="37"/>
+      <c r="D95" s="37"/>
+      <c r="E95" s="37"/>
+      <c r="F95" s="37"/>
+      <c r="G95" s="37"/>
+      <c r="H95" s="37"/>
+      <c r="I95" s="37"/>
+      <c r="J95" s="37"/>
     </row>
     <row r="96" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B96" s="36"/>
-      <c r="C96" s="36"/>
-      <c r="D96" s="36"/>
-      <c r="E96" s="36"/>
-      <c r="F96" s="36"/>
-      <c r="G96" s="36"/>
-      <c r="H96" s="36"/>
-      <c r="I96" s="36"/>
-      <c r="J96" s="36"/>
+      <c r="B96" s="37"/>
+      <c r="C96" s="37"/>
+      <c r="D96" s="37"/>
+      <c r="E96" s="37"/>
+      <c r="F96" s="37"/>
+      <c r="G96" s="37"/>
+      <c r="H96" s="37"/>
+      <c r="I96" s="37"/>
+      <c r="J96" s="37"/>
     </row>
     <row r="97" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B97" s="36"/>
-      <c r="C97" s="36"/>
-      <c r="D97" s="36"/>
-      <c r="E97" s="36"/>
-      <c r="F97" s="36"/>
-      <c r="G97" s="36"/>
-      <c r="H97" s="36"/>
-      <c r="I97" s="36"/>
-      <c r="J97" s="36"/>
+      <c r="B97" s="37"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="37"/>
+      <c r="F97" s="37"/>
+      <c r="G97" s="37"/>
+      <c r="H97" s="37"/>
+      <c r="I97" s="37"/>
+      <c r="J97" s="37"/>
     </row>
     <row r="98" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B98" s="36"/>
-      <c r="C98" s="36"/>
-      <c r="D98" s="36"/>
-      <c r="E98" s="36"/>
-      <c r="F98" s="36"/>
-      <c r="G98" s="36"/>
-      <c r="H98" s="36"/>
-      <c r="I98" s="36"/>
-      <c r="J98" s="36"/>
+      <c r="B98" s="37"/>
+      <c r="C98" s="37"/>
+      <c r="D98" s="37"/>
+      <c r="E98" s="37"/>
+      <c r="F98" s="37"/>
+      <c r="G98" s="37"/>
+      <c r="H98" s="37"/>
+      <c r="I98" s="37"/>
+      <c r="J98" s="37"/>
     </row>
     <row r="99" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B99" s="36"/>
-      <c r="C99" s="36"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="36"/>
-      <c r="F99" s="36"/>
-      <c r="G99" s="36"/>
-      <c r="H99" s="36"/>
-      <c r="I99" s="36"/>
-      <c r="J99" s="36"/>
+      <c r="B99" s="37"/>
+      <c r="C99" s="37"/>
+      <c r="D99" s="37"/>
+      <c r="E99" s="37"/>
+      <c r="F99" s="37"/>
+      <c r="G99" s="37"/>
+      <c r="H99" s="37"/>
+      <c r="I99" s="37"/>
+      <c r="J99" s="37"/>
     </row>
     <row r="100" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B100" s="36"/>
-      <c r="C100" s="36"/>
-      <c r="D100" s="36"/>
-      <c r="E100" s="36"/>
-      <c r="F100" s="36"/>
-      <c r="G100" s="36"/>
-      <c r="H100" s="36"/>
-      <c r="I100" s="36"/>
-      <c r="J100" s="36"/>
+      <c r="B100" s="37"/>
+      <c r="C100" s="37"/>
+      <c r="D100" s="37"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="37"/>
+      <c r="G100" s="37"/>
+      <c r="H100" s="37"/>
+      <c r="I100" s="37"/>
+      <c r="J100" s="37"/>
     </row>
     <row r="101" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B101" s="36"/>
-      <c r="C101" s="36"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
-      <c r="F101" s="36"/>
-      <c r="G101" s="36"/>
-      <c r="H101" s="36"/>
-      <c r="I101" s="36"/>
-      <c r="J101" s="36"/>
+      <c r="B101" s="37"/>
+      <c r="C101" s="37"/>
+      <c r="D101" s="37"/>
+      <c r="E101" s="37"/>
+      <c r="F101" s="37"/>
+      <c r="G101" s="37"/>
+      <c r="H101" s="37"/>
+      <c r="I101" s="37"/>
+      <c r="J101" s="37"/>
     </row>
     <row r="102" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B102" s="36"/>
-      <c r="C102" s="36"/>
-      <c r="D102" s="36"/>
-      <c r="E102" s="36"/>
-      <c r="F102" s="36"/>
-      <c r="G102" s="36"/>
-      <c r="H102" s="36"/>
-      <c r="I102" s="36"/>
-      <c r="J102" s="36"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="37"/>
+      <c r="D102" s="37"/>
+      <c r="E102" s="37"/>
+      <c r="F102" s="37"/>
+      <c r="G102" s="37"/>
+      <c r="H102" s="37"/>
+      <c r="I102" s="37"/>
+      <c r="J102" s="37"/>
     </row>
     <row r="103" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B103" s="36"/>
-      <c r="C103" s="36"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="36"/>
-      <c r="F103" s="36"/>
-      <c r="G103" s="36"/>
-      <c r="H103" s="36"/>
-      <c r="I103" s="36"/>
-      <c r="J103" s="36"/>
+      <c r="B103" s="37"/>
+      <c r="C103" s="37"/>
+      <c r="D103" s="37"/>
+      <c r="E103" s="37"/>
+      <c r="F103" s="37"/>
+      <c r="G103" s="37"/>
+      <c r="H103" s="37"/>
+      <c r="I103" s="37"/>
+      <c r="J103" s="37"/>
     </row>
     <row r="104" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B104" s="36"/>
-      <c r="C104" s="36"/>
-      <c r="D104" s="36"/>
-      <c r="E104" s="36"/>
-      <c r="F104" s="36"/>
-      <c r="G104" s="36"/>
-      <c r="H104" s="36"/>
-      <c r="I104" s="36"/>
-      <c r="J104" s="36"/>
+      <c r="B104" s="37"/>
+      <c r="C104" s="37"/>
+      <c r="D104" s="37"/>
+      <c r="E104" s="37"/>
+      <c r="F104" s="37"/>
+      <c r="G104" s="37"/>
+      <c r="H104" s="37"/>
+      <c r="I104" s="37"/>
+      <c r="J104" s="37"/>
     </row>
     <row r="105" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B105" s="36"/>
-      <c r="C105" s="36"/>
-      <c r="D105" s="36"/>
-      <c r="E105" s="36"/>
-      <c r="F105" s="36"/>
-      <c r="G105" s="36"/>
-      <c r="H105" s="36"/>
-      <c r="I105" s="36"/>
-      <c r="J105" s="36"/>
+      <c r="B105" s="37"/>
+      <c r="C105" s="37"/>
+      <c r="D105" s="37"/>
+      <c r="E105" s="37"/>
+      <c r="F105" s="37"/>
+      <c r="G105" s="37"/>
+      <c r="H105" s="37"/>
+      <c r="I105" s="37"/>
+      <c r="J105" s="37"/>
     </row>
     <row r="106" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B106" s="36"/>
-      <c r="C106" s="36"/>
-      <c r="D106" s="36"/>
-      <c r="E106" s="36"/>
-      <c r="F106" s="36"/>
-      <c r="G106" s="36"/>
-      <c r="H106" s="36"/>
-      <c r="I106" s="36"/>
-      <c r="J106" s="36"/>
+      <c r="B106" s="37"/>
+      <c r="C106" s="37"/>
+      <c r="D106" s="37"/>
+      <c r="E106" s="37"/>
+      <c r="F106" s="37"/>
+      <c r="G106" s="37"/>
+      <c r="H106" s="37"/>
+      <c r="I106" s="37"/>
+      <c r="J106" s="37"/>
     </row>
     <row r="107" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B107" s="36"/>
-      <c r="C107" s="36"/>
-      <c r="D107" s="36"/>
-      <c r="E107" s="36"/>
-      <c r="F107" s="36"/>
-      <c r="G107" s="36"/>
-      <c r="H107" s="36"/>
-      <c r="I107" s="36"/>
-      <c r="J107" s="36"/>
+      <c r="B107" s="37"/>
+      <c r="C107" s="37"/>
+      <c r="D107" s="37"/>
+      <c r="E107" s="37"/>
+      <c r="F107" s="37"/>
+      <c r="G107" s="37"/>
+      <c r="H107" s="37"/>
+      <c r="I107" s="37"/>
+      <c r="J107" s="37"/>
     </row>
     <row r="108" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B108" s="36"/>
-      <c r="C108" s="36"/>
-      <c r="D108" s="36"/>
-      <c r="E108" s="36"/>
-      <c r="F108" s="36"/>
-      <c r="G108" s="36"/>
-      <c r="H108" s="36"/>
-      <c r="I108" s="36"/>
-      <c r="J108" s="36"/>
+      <c r="B108" s="37"/>
+      <c r="C108" s="37"/>
+      <c r="D108" s="37"/>
+      <c r="E108" s="37"/>
+      <c r="F108" s="37"/>
+      <c r="G108" s="37"/>
+      <c r="H108" s="37"/>
+      <c r="I108" s="37"/>
+      <c r="J108" s="37"/>
     </row>
     <row r="109" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B109" s="36"/>
-      <c r="C109" s="36"/>
-      <c r="D109" s="36"/>
-      <c r="E109" s="36"/>
-      <c r="F109" s="36"/>
-      <c r="G109" s="36"/>
-      <c r="H109" s="36"/>
-      <c r="I109" s="36"/>
-      <c r="J109" s="36"/>
+      <c r="B109" s="37"/>
+      <c r="C109" s="37"/>
+      <c r="D109" s="37"/>
+      <c r="E109" s="37"/>
+      <c r="F109" s="37"/>
+      <c r="G109" s="37"/>
+      <c r="H109" s="37"/>
+      <c r="I109" s="37"/>
+      <c r="J109" s="37"/>
     </row>
     <row r="110" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B110" s="36"/>
-      <c r="C110" s="36"/>
-      <c r="D110" s="36"/>
-      <c r="E110" s="36"/>
-      <c r="F110" s="36"/>
-      <c r="G110" s="36"/>
-      <c r="H110" s="36"/>
-      <c r="I110" s="36"/>
-      <c r="J110" s="36"/>
+      <c r="B110" s="37"/>
+      <c r="C110" s="37"/>
+      <c r="D110" s="37"/>
+      <c r="E110" s="37"/>
+      <c r="F110" s="37"/>
+      <c r="G110" s="37"/>
+      <c r="H110" s="37"/>
+      <c r="I110" s="37"/>
+      <c r="J110" s="37"/>
     </row>
     <row r="111" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B111" s="36"/>
-      <c r="C111" s="36"/>
-      <c r="D111" s="36"/>
-      <c r="E111" s="36"/>
-      <c r="F111" s="36"/>
-      <c r="G111" s="36"/>
-      <c r="H111" s="36"/>
-      <c r="I111" s="36"/>
-      <c r="J111" s="36"/>
+      <c r="B111" s="37"/>
+      <c r="C111" s="37"/>
+      <c r="D111" s="37"/>
+      <c r="E111" s="37"/>
+      <c r="F111" s="37"/>
+      <c r="G111" s="37"/>
+      <c r="H111" s="37"/>
+      <c r="I111" s="37"/>
+      <c r="J111" s="37"/>
     </row>
     <row r="112" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B112" s="36"/>
-      <c r="C112" s="36"/>
-      <c r="D112" s="36"/>
-      <c r="E112" s="36"/>
-      <c r="F112" s="36"/>
-      <c r="G112" s="36"/>
-      <c r="H112" s="36"/>
-      <c r="I112" s="36"/>
-      <c r="J112" s="36"/>
+      <c r="B112" s="37"/>
+      <c r="C112" s="37"/>
+      <c r="D112" s="37"/>
+      <c r="E112" s="37"/>
+      <c r="F112" s="37"/>
+      <c r="G112" s="37"/>
+      <c r="H112" s="37"/>
+      <c r="I112" s="37"/>
+      <c r="J112" s="37"/>
     </row>
     <row r="113" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B113" s="36"/>
-      <c r="C113" s="36"/>
-      <c r="D113" s="36"/>
-      <c r="E113" s="36"/>
-      <c r="F113" s="36"/>
-      <c r="G113" s="36"/>
-      <c r="H113" s="36"/>
-      <c r="I113" s="36"/>
-      <c r="J113" s="36"/>
+      <c r="B113" s="37"/>
+      <c r="C113" s="37"/>
+      <c r="D113" s="37"/>
+      <c r="E113" s="37"/>
+      <c r="F113" s="37"/>
+      <c r="G113" s="37"/>
+      <c r="H113" s="37"/>
+      <c r="I113" s="37"/>
+      <c r="J113" s="37"/>
     </row>
     <row r="114" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B114" s="36"/>
-      <c r="C114" s="36"/>
-      <c r="D114" s="36"/>
-      <c r="E114" s="36"/>
-      <c r="F114" s="36"/>
-      <c r="G114" s="36"/>
-      <c r="H114" s="36"/>
-      <c r="I114" s="36"/>
-      <c r="J114" s="36"/>
+      <c r="B114" s="37"/>
+      <c r="C114" s="37"/>
+      <c r="D114" s="37"/>
+      <c r="E114" s="37"/>
+      <c r="F114" s="37"/>
+      <c r="G114" s="37"/>
+      <c r="H114" s="37"/>
+      <c r="I114" s="37"/>
+      <c r="J114" s="37"/>
     </row>
     <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B115" s="36"/>
-      <c r="C115" s="36"/>
-      <c r="D115" s="36"/>
-      <c r="E115" s="36"/>
-      <c r="F115" s="36"/>
-      <c r="G115" s="36"/>
-      <c r="H115" s="36"/>
-      <c r="I115" s="36"/>
-      <c r="J115" s="36"/>
+      <c r="B115" s="37"/>
+      <c r="C115" s="37"/>
+      <c r="D115" s="37"/>
+      <c r="E115" s="37"/>
+      <c r="F115" s="37"/>
+      <c r="G115" s="37"/>
+      <c r="H115" s="37"/>
+      <c r="I115" s="37"/>
+      <c r="J115" s="37"/>
     </row>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B116" s="36"/>
-      <c r="C116" s="36"/>
-      <c r="D116" s="36"/>
-      <c r="E116" s="36"/>
-      <c r="F116" s="36"/>
-      <c r="G116" s="36"/>
-      <c r="H116" s="36"/>
-      <c r="I116" s="36"/>
-      <c r="J116" s="36"/>
+      <c r="B116" s="37"/>
+      <c r="C116" s="37"/>
+      <c r="D116" s="37"/>
+      <c r="E116" s="37"/>
+      <c r="F116" s="37"/>
+      <c r="G116" s="37"/>
+      <c r="H116" s="37"/>
+      <c r="I116" s="37"/>
+      <c r="J116" s="37"/>
     </row>
     <row r="117" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="118" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B118" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="C118" s="36"/>
-      <c r="D118" s="36"/>
-      <c r="E118" s="36"/>
-      <c r="F118" s="36"/>
-      <c r="G118" s="36"/>
-      <c r="H118" s="36"/>
-      <c r="I118" s="36"/>
-      <c r="J118" s="36"/>
+      <c r="B118" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C118" s="37"/>
+      <c r="D118" s="37"/>
+      <c r="E118" s="37"/>
+      <c r="F118" s="37"/>
+      <c r="G118" s="37"/>
+      <c r="H118" s="37"/>
+      <c r="I118" s="37"/>
+      <c r="J118" s="37"/>
     </row>
     <row r="119" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B119" s="36"/>
-      <c r="C119" s="36"/>
-      <c r="D119" s="36"/>
-      <c r="E119" s="36"/>
-      <c r="F119" s="36"/>
-      <c r="G119" s="36"/>
-      <c r="H119" s="36"/>
-      <c r="I119" s="36"/>
-      <c r="J119" s="36"/>
+      <c r="B119" s="37"/>
+      <c r="C119" s="37"/>
+      <c r="D119" s="37"/>
+      <c r="E119" s="37"/>
+      <c r="F119" s="37"/>
+      <c r="G119" s="37"/>
+      <c r="H119" s="37"/>
+      <c r="I119" s="37"/>
+      <c r="J119" s="37"/>
     </row>
     <row r="120" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B120" s="36"/>
-      <c r="C120" s="36"/>
-      <c r="D120" s="36"/>
-      <c r="E120" s="36"/>
-      <c r="F120" s="36"/>
-      <c r="G120" s="36"/>
-      <c r="H120" s="36"/>
-      <c r="I120" s="36"/>
-      <c r="J120" s="36"/>
+      <c r="B120" s="37"/>
+      <c r="C120" s="37"/>
+      <c r="D120" s="37"/>
+      <c r="E120" s="37"/>
+      <c r="F120" s="37"/>
+      <c r="G120" s="37"/>
+      <c r="H120" s="37"/>
+      <c r="I120" s="37"/>
+      <c r="J120" s="37"/>
     </row>
     <row r="121" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B121" s="36"/>
-      <c r="C121" s="36"/>
-      <c r="D121" s="36"/>
-      <c r="E121" s="36"/>
-      <c r="F121" s="36"/>
-      <c r="G121" s="36"/>
-      <c r="H121" s="36"/>
-      <c r="I121" s="36"/>
-      <c r="J121" s="36"/>
+      <c r="B121" s="37"/>
+      <c r="C121" s="37"/>
+      <c r="D121" s="37"/>
+      <c r="E121" s="37"/>
+      <c r="F121" s="37"/>
+      <c r="G121" s="37"/>
+      <c r="H121" s="37"/>
+      <c r="I121" s="37"/>
+      <c r="J121" s="37"/>
     </row>
     <row r="122" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B122" s="36"/>
-      <c r="C122" s="36"/>
-      <c r="D122" s="36"/>
-      <c r="E122" s="36"/>
-      <c r="F122" s="36"/>
-      <c r="G122" s="36"/>
-      <c r="H122" s="36"/>
-      <c r="I122" s="36"/>
-      <c r="J122" s="36"/>
+      <c r="B122" s="37"/>
+      <c r="C122" s="37"/>
+      <c r="D122" s="37"/>
+      <c r="E122" s="37"/>
+      <c r="F122" s="37"/>
+      <c r="G122" s="37"/>
+      <c r="H122" s="37"/>
+      <c r="I122" s="37"/>
+      <c r="J122" s="37"/>
     </row>
     <row r="123" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B123" s="36"/>
-      <c r="C123" s="36"/>
-      <c r="D123" s="36"/>
-      <c r="E123" s="36"/>
-      <c r="F123" s="36"/>
-      <c r="G123" s="36"/>
-      <c r="H123" s="36"/>
-      <c r="I123" s="36"/>
-      <c r="J123" s="36"/>
+      <c r="B123" s="37"/>
+      <c r="C123" s="37"/>
+      <c r="D123" s="37"/>
+      <c r="E123" s="37"/>
+      <c r="F123" s="37"/>
+      <c r="G123" s="37"/>
+      <c r="H123" s="37"/>
+      <c r="I123" s="37"/>
+      <c r="J123" s="37"/>
     </row>
     <row r="124" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B124" s="36"/>
-      <c r="C124" s="36"/>
-      <c r="D124" s="36"/>
-      <c r="E124" s="36"/>
-      <c r="F124" s="36"/>
-      <c r="G124" s="36"/>
-      <c r="H124" s="36"/>
-      <c r="I124" s="36"/>
-      <c r="J124" s="36"/>
+      <c r="B124" s="37"/>
+      <c r="C124" s="37"/>
+      <c r="D124" s="37"/>
+      <c r="E124" s="37"/>
+      <c r="F124" s="37"/>
+      <c r="G124" s="37"/>
+      <c r="H124" s="37"/>
+      <c r="I124" s="37"/>
+      <c r="J124" s="37"/>
     </row>
     <row r="125" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B125" s="36"/>
-      <c r="C125" s="36"/>
-      <c r="D125" s="36"/>
-      <c r="E125" s="36"/>
-      <c r="F125" s="36"/>
-      <c r="G125" s="36"/>
-      <c r="H125" s="36"/>
-      <c r="I125" s="36"/>
-      <c r="J125" s="36"/>
+      <c r="B125" s="37"/>
+      <c r="C125" s="37"/>
+      <c r="D125" s="37"/>
+      <c r="E125" s="37"/>
+      <c r="F125" s="37"/>
+      <c r="G125" s="37"/>
+      <c r="H125" s="37"/>
+      <c r="I125" s="37"/>
+      <c r="J125" s="37"/>
     </row>
     <row r="126" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B126" s="36"/>
-      <c r="C126" s="36"/>
-      <c r="D126" s="36"/>
-      <c r="E126" s="36"/>
-      <c r="F126" s="36"/>
-      <c r="G126" s="36"/>
-      <c r="H126" s="36"/>
-      <c r="I126" s="36"/>
-      <c r="J126" s="36"/>
+      <c r="B126" s="37"/>
+      <c r="C126" s="37"/>
+      <c r="D126" s="37"/>
+      <c r="E126" s="37"/>
+      <c r="F126" s="37"/>
+      <c r="G126" s="37"/>
+      <c r="H126" s="37"/>
+      <c r="I126" s="37"/>
+      <c r="J126" s="37"/>
     </row>
     <row r="127" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B127" s="36"/>
-      <c r="C127" s="36"/>
-      <c r="D127" s="36"/>
-      <c r="E127" s="36"/>
-      <c r="F127" s="36"/>
-      <c r="G127" s="36"/>
-      <c r="H127" s="36"/>
-      <c r="I127" s="36"/>
-      <c r="J127" s="36"/>
+      <c r="B127" s="37"/>
+      <c r="C127" s="37"/>
+      <c r="D127" s="37"/>
+      <c r="E127" s="37"/>
+      <c r="F127" s="37"/>
+      <c r="G127" s="37"/>
+      <c r="H127" s="37"/>
+      <c r="I127" s="37"/>
+      <c r="J127" s="37"/>
     </row>
     <row r="128" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B128" s="36"/>
-      <c r="C128" s="36"/>
-      <c r="D128" s="36"/>
-      <c r="E128" s="36"/>
-      <c r="F128" s="36"/>
-      <c r="G128" s="36"/>
-      <c r="H128" s="36"/>
-      <c r="I128" s="36"/>
-      <c r="J128" s="36"/>
+      <c r="B128" s="37"/>
+      <c r="C128" s="37"/>
+      <c r="D128" s="37"/>
+      <c r="E128" s="37"/>
+      <c r="F128" s="37"/>
+      <c r="G128" s="37"/>
+      <c r="H128" s="37"/>
+      <c r="I128" s="37"/>
+      <c r="J128" s="37"/>
     </row>
     <row r="129" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B129" s="36"/>
-      <c r="C129" s="36"/>
-      <c r="D129" s="36"/>
-      <c r="E129" s="36"/>
-      <c r="F129" s="36"/>
-      <c r="G129" s="36"/>
-      <c r="H129" s="36"/>
-      <c r="I129" s="36"/>
-      <c r="J129" s="36"/>
+      <c r="B129" s="37"/>
+      <c r="C129" s="37"/>
+      <c r="D129" s="37"/>
+      <c r="E129" s="37"/>
+      <c r="F129" s="37"/>
+      <c r="G129" s="37"/>
+      <c r="H129" s="37"/>
+      <c r="I129" s="37"/>
+      <c r="J129" s="37"/>
     </row>
     <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B130" s="36"/>
-      <c r="C130" s="36"/>
-      <c r="D130" s="36"/>
-      <c r="E130" s="36"/>
-      <c r="F130" s="36"/>
-      <c r="G130" s="36"/>
-      <c r="H130" s="36"/>
-      <c r="I130" s="36"/>
-      <c r="J130" s="36"/>
+      <c r="B130" s="37"/>
+      <c r="C130" s="37"/>
+      <c r="D130" s="37"/>
+      <c r="E130" s="37"/>
+      <c r="F130" s="37"/>
+      <c r="G130" s="37"/>
+      <c r="H130" s="37"/>
+      <c r="I130" s="37"/>
+      <c r="J130" s="37"/>
     </row>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B131" s="36"/>
-      <c r="C131" s="36"/>
-      <c r="D131" s="36"/>
-      <c r="E131" s="36"/>
-      <c r="F131" s="36"/>
-      <c r="G131" s="36"/>
-      <c r="H131" s="36"/>
-      <c r="I131" s="36"/>
-      <c r="J131" s="36"/>
+      <c r="B131" s="37"/>
+      <c r="C131" s="37"/>
+      <c r="D131" s="37"/>
+      <c r="E131" s="37"/>
+      <c r="F131" s="37"/>
+      <c r="G131" s="37"/>
+      <c r="H131" s="37"/>
+      <c r="I131" s="37"/>
+      <c r="J131" s="37"/>
     </row>
     <row r="132" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="133" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B133" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C133" s="36"/>
-      <c r="D133" s="36"/>
-      <c r="E133" s="36"/>
-      <c r="F133" s="36"/>
-      <c r="G133" s="36"/>
-      <c r="H133" s="36"/>
-      <c r="I133" s="36"/>
-      <c r="J133" s="36"/>
+      <c r="B133" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C133" s="37"/>
+      <c r="D133" s="37"/>
+      <c r="E133" s="37"/>
+      <c r="F133" s="37"/>
+      <c r="G133" s="37"/>
+      <c r="H133" s="37"/>
+      <c r="I133" s="37"/>
+      <c r="J133" s="37"/>
     </row>
     <row r="134" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B134" s="36"/>
-      <c r="C134" s="36"/>
-      <c r="D134" s="36"/>
-      <c r="E134" s="36"/>
-      <c r="F134" s="36"/>
-      <c r="G134" s="36"/>
-      <c r="H134" s="36"/>
-      <c r="I134" s="36"/>
-      <c r="J134" s="36"/>
+      <c r="B134" s="37"/>
+      <c r="C134" s="37"/>
+      <c r="D134" s="37"/>
+      <c r="E134" s="37"/>
+      <c r="F134" s="37"/>
+      <c r="G134" s="37"/>
+      <c r="H134" s="37"/>
+      <c r="I134" s="37"/>
+      <c r="J134" s="37"/>
     </row>
     <row r="135" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B135" s="36"/>
-      <c r="C135" s="36"/>
-      <c r="D135" s="36"/>
-      <c r="E135" s="36"/>
-      <c r="F135" s="36"/>
-      <c r="G135" s="36"/>
-      <c r="H135" s="36"/>
-      <c r="I135" s="36"/>
-      <c r="J135" s="36"/>
+      <c r="B135" s="37"/>
+      <c r="C135" s="37"/>
+      <c r="D135" s="37"/>
+      <c r="E135" s="37"/>
+      <c r="F135" s="37"/>
+      <c r="G135" s="37"/>
+      <c r="H135" s="37"/>
+      <c r="I135" s="37"/>
+      <c r="J135" s="37"/>
     </row>
     <row r="136" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B136" s="36"/>
-      <c r="C136" s="36"/>
-      <c r="D136" s="36"/>
-      <c r="E136" s="36"/>
-      <c r="F136" s="36"/>
-      <c r="G136" s="36"/>
-      <c r="H136" s="36"/>
-      <c r="I136" s="36"/>
-      <c r="J136" s="36"/>
+      <c r="B136" s="37"/>
+      <c r="C136" s="37"/>
+      <c r="D136" s="37"/>
+      <c r="E136" s="37"/>
+      <c r="F136" s="37"/>
+      <c r="G136" s="37"/>
+      <c r="H136" s="37"/>
+      <c r="I136" s="37"/>
+      <c r="J136" s="37"/>
     </row>
     <row r="137" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B137" s="36"/>
-      <c r="C137" s="36"/>
-      <c r="D137" s="36"/>
-      <c r="E137" s="36"/>
-      <c r="F137" s="36"/>
-      <c r="G137" s="36"/>
-      <c r="H137" s="36"/>
-      <c r="I137" s="36"/>
-      <c r="J137" s="36"/>
+      <c r="B137" s="37"/>
+      <c r="C137" s="37"/>
+      <c r="D137" s="37"/>
+      <c r="E137" s="37"/>
+      <c r="F137" s="37"/>
+      <c r="G137" s="37"/>
+      <c r="H137" s="37"/>
+      <c r="I137" s="37"/>
+      <c r="J137" s="37"/>
     </row>
     <row r="138" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B138" s="36"/>
-      <c r="C138" s="36"/>
-      <c r="D138" s="36"/>
-      <c r="E138" s="36"/>
-      <c r="F138" s="36"/>
-      <c r="G138" s="36"/>
-      <c r="H138" s="36"/>
-      <c r="I138" s="36"/>
-      <c r="J138" s="36"/>
+      <c r="B138" s="37"/>
+      <c r="C138" s="37"/>
+      <c r="D138" s="37"/>
+      <c r="E138" s="37"/>
+      <c r="F138" s="37"/>
+      <c r="G138" s="37"/>
+      <c r="H138" s="37"/>
+      <c r="I138" s="37"/>
+      <c r="J138" s="37"/>
     </row>
     <row r="139" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B139" s="36"/>
-      <c r="C139" s="36"/>
-      <c r="D139" s="36"/>
-      <c r="E139" s="36"/>
-      <c r="F139" s="36"/>
-      <c r="G139" s="36"/>
-      <c r="H139" s="36"/>
-      <c r="I139" s="36"/>
-      <c r="J139" s="36"/>
+      <c r="B139" s="37"/>
+      <c r="C139" s="37"/>
+      <c r="D139" s="37"/>
+      <c r="E139" s="37"/>
+      <c r="F139" s="37"/>
+      <c r="G139" s="37"/>
+      <c r="H139" s="37"/>
+      <c r="I139" s="37"/>
+      <c r="J139" s="37"/>
     </row>
     <row r="140" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B140" s="36"/>
-      <c r="C140" s="36"/>
-      <c r="D140" s="36"/>
-      <c r="E140" s="36"/>
-      <c r="F140" s="36"/>
-      <c r="G140" s="36"/>
-      <c r="H140" s="36"/>
-      <c r="I140" s="36"/>
-      <c r="J140" s="36"/>
+      <c r="B140" s="37"/>
+      <c r="C140" s="37"/>
+      <c r="D140" s="37"/>
+      <c r="E140" s="37"/>
+      <c r="F140" s="37"/>
+      <c r="G140" s="37"/>
+      <c r="H140" s="37"/>
+      <c r="I140" s="37"/>
+      <c r="J140" s="37"/>
     </row>
     <row r="141" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B141" s="36"/>
-      <c r="C141" s="36"/>
-      <c r="D141" s="36"/>
-      <c r="E141" s="36"/>
-      <c r="F141" s="36"/>
-      <c r="G141" s="36"/>
-      <c r="H141" s="36"/>
-      <c r="I141" s="36"/>
-      <c r="J141" s="36"/>
+      <c r="B141" s="37"/>
+      <c r="C141" s="37"/>
+      <c r="D141" s="37"/>
+      <c r="E141" s="37"/>
+      <c r="F141" s="37"/>
+      <c r="G141" s="37"/>
+      <c r="H141" s="37"/>
+      <c r="I141" s="37"/>
+      <c r="J141" s="37"/>
     </row>
     <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B143" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="C143" s="38"/>
-      <c r="D143" s="38"/>
-      <c r="E143" s="38"/>
-      <c r="F143" s="38"/>
-      <c r="G143" s="38"/>
-      <c r="H143" s="38"/>
-      <c r="I143" s="38"/>
-      <c r="J143" s="38"/>
+      <c r="B143" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C143" s="39"/>
+      <c r="D143" s="39"/>
+      <c r="E143" s="39"/>
+      <c r="F143" s="39"/>
+      <c r="G143" s="39"/>
+      <c r="H143" s="39"/>
+      <c r="I143" s="39"/>
+      <c r="J143" s="39"/>
     </row>
     <row r="144" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B144" s="38"/>
-      <c r="C144" s="38"/>
-      <c r="D144" s="38"/>
-      <c r="E144" s="38"/>
-      <c r="F144" s="38"/>
-      <c r="G144" s="38"/>
-      <c r="H144" s="38"/>
-      <c r="I144" s="38"/>
-      <c r="J144" s="38"/>
+      <c r="B144" s="39"/>
+      <c r="C144" s="39"/>
+      <c r="D144" s="39"/>
+      <c r="E144" s="39"/>
+      <c r="F144" s="39"/>
+      <c r="G144" s="39"/>
+      <c r="H144" s="39"/>
+      <c r="I144" s="39"/>
+      <c r="J144" s="39"/>
     </row>
     <row r="145" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B145" s="38"/>
-      <c r="C145" s="38"/>
-      <c r="D145" s="38"/>
-      <c r="E145" s="38"/>
-      <c r="F145" s="38"/>
-      <c r="G145" s="38"/>
-      <c r="H145" s="38"/>
-      <c r="I145" s="38"/>
-      <c r="J145" s="38"/>
+      <c r="B145" s="39"/>
+      <c r="C145" s="39"/>
+      <c r="D145" s="39"/>
+      <c r="E145" s="39"/>
+      <c r="F145" s="39"/>
+      <c r="G145" s="39"/>
+      <c r="H145" s="39"/>
+      <c r="I145" s="39"/>
+      <c r="J145" s="39"/>
     </row>
     <row r="146" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B146" s="38"/>
-      <c r="C146" s="38"/>
-      <c r="D146" s="38"/>
-      <c r="E146" s="38"/>
-      <c r="F146" s="38"/>
-      <c r="G146" s="38"/>
-      <c r="H146" s="38"/>
-      <c r="I146" s="38"/>
-      <c r="J146" s="38"/>
+      <c r="B146" s="39"/>
+      <c r="C146" s="39"/>
+      <c r="D146" s="39"/>
+      <c r="E146" s="39"/>
+      <c r="F146" s="39"/>
+      <c r="G146" s="39"/>
+      <c r="H146" s="39"/>
+      <c r="I146" s="39"/>
+      <c r="J146" s="39"/>
     </row>
     <row r="147" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B147" s="38"/>
-      <c r="C147" s="38"/>
-      <c r="D147" s="38"/>
-      <c r="E147" s="38"/>
-      <c r="F147" s="38"/>
-      <c r="G147" s="38"/>
-      <c r="H147" s="38"/>
-      <c r="I147" s="38"/>
-      <c r="J147" s="38"/>
+      <c r="B147" s="39"/>
+      <c r="C147" s="39"/>
+      <c r="D147" s="39"/>
+      <c r="E147" s="39"/>
+      <c r="F147" s="39"/>
+      <c r="G147" s="39"/>
+      <c r="H147" s="39"/>
+      <c r="I147" s="39"/>
+      <c r="J147" s="39"/>
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D148" s="17" t="s">
+      <c r="D148" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E148" s="35" t="s">
+      <c r="E148" s="34" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5205,9 +5210,9 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" xr:uid="{FF66E5E8-E35C-40A8-934B-0F626EB9EC1C}"/>
-    <hyperlink ref="D9" r:id="rId2" xr:uid="{077364E9-60BE-4408-B788-07097A8660A6}"/>
-    <hyperlink ref="E148" r:id="rId3" xr:uid="{F794EFA8-DA6C-4550-9380-2FD01C44324D}"/>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{30E33FA8-2170-4C69-B1B0-A9334974B6B8}"/>
+    <hyperlink ref="D9" r:id="rId2" xr:uid="{723567C3-7EAE-4AE6-ACF1-605C40A24E6E}"/>
+    <hyperlink ref="E148" r:id="rId3" xr:uid="{FDC1B3A0-CED8-4AB3-B835-FAF0C3C949BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -5222,7 +5227,7 @@
   <dimension ref="A1:D994"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5234,153 +5239,153 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="A13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6378,8 +6383,8 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6396,60 +6401,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="23" t="s">
+      <c r="G2" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="31"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="31"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6478,45 +6483,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6991,7 +6996,7 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -7005,40 +7010,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7067,20 +7072,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>